<commit_message>
add Tesseract OCR for unreadable pdf files
</commit_message>
<xml_diff>
--- a/data/result/result.xlsx
+++ b/data/result/result.xlsx
@@ -456,15 +456,15 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>нефтеотдача</t>
+          <t>почва</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.3288214439537894</v>
+        <v>0.3885720750025864</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>конечный нефтеотдача, нефтеотдача пласт, повышение нефтеотдача, фактор влиять нефтеотдача</t>
+          <t>устойчивость почва, почва грунт, режим почва, самоочищение почва</t>
         </is>
       </c>
     </row>
@@ -474,15 +474,15 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>пласт</t>
+          <t>загрязнение</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.2020149243149546</v>
+        <v>0.180935045705758</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>нефтеотдача пласт, коэффициент охват пласт, извлечь пласт, количество извлечь пласт</t>
+          <t>нефтяной загрязнение, источник загрязнение, ореол загрязнение, ореол нефтяной загрязнение</t>
         </is>
       </c>
     </row>
@@ -492,15 +492,15 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>нефть</t>
+          <t>ландшафт</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.178806955663011</v>
+        <v>0.1449324059469544</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>добыча нефть, вязкость нефть, извлечь пласт нефть, нефть пласт</t>
+          <t>компонент ландшафт, ландшафтно геохимический, ландшафтно, состояние ландшафт</t>
         </is>
       </c>
     </row>
@@ -510,15 +510,15 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>заводнение</t>
+          <t>геохимический</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.1141403809079946</v>
+        <v>0.1381817999887385</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>охват залежь заводнение, залежь заводнение, заводнение коэффициент, заводнение коэффициент охват</t>
+          <t>эколого геохимический, эколого геохимический карта, геохимический поле, ландшафтно геохимический</t>
         </is>
       </c>
     </row>
@@ -528,15 +528,15 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>коэффициент охват</t>
+          <t>поллютант</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.1053887189256356</v>
+        <v>0.1365767393522176</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>коэффициент охват пласт, заводнение коэффициент охват, коэффициент охват залежь, вытеснение коэффициент охват</t>
+          <t>поллютант природный</t>
         </is>
       </c>
     </row>
@@ -546,15 +546,15 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>конечный нефтеотдача</t>
+          <t>почвенный</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.09660839118374866</v>
+        <v>0.1084635580499261</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>конечный нефтеотдача текущий</t>
+          <t>почвенный покров, почвенный экосистема</t>
         </is>
       </c>
     </row>
@@ -564,17 +564,13 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>отношение количество</t>
+          <t>моск ун тот</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.09550296149496046</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>нефтеотдача отношение количество, отношение количество извлечь</t>
-        </is>
-      </c>
+        <v>0.1037261012262532</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -582,15 +578,15 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>коэффициент</t>
+          <t>моск ун</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.09237775791152383</v>
+        <v>0.1037261012262532</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>коэффициент охват, коэффициент вытеснение, коэффициент охват пласт, коэффициент вытеснение коэффициент</t>
+          <t>моск ун тот, вестн моск ун, во моск ун</t>
         </is>
       </c>
     </row>
@@ -600,15 +596,15 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>нефтеотдача пласт</t>
+          <t>моск</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.09076514308339242</v>
+        <v>0.09752222461185295</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>повышение нефтеотдача пласт</t>
+          <t>моск ун тот, моск ун, вестн моск, вестн моск ун</t>
         </is>
       </c>
     </row>
@@ -618,15 +614,15 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>недра</t>
+          <t>география</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.08559366195950284</v>
+        <v>0.09589309825489614</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>недра муравей, недра казак</t>
+          <t>сера география, тот сера география</t>
         </is>
       </c>
     </row>
@@ -636,15 +632,15 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>охват</t>
+          <t>техногенный</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.08497771763711093</v>
+        <v>0.0955063826114305</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>коэффициент охват, коэффициент охват пласт, охват пласт, охватить</t>
+          <t>техногенный углеводород, техногенный поток, техногенный поток углеводород, природный техногенный</t>
         </is>
       </c>
     </row>
@@ -654,15 +650,15 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>коэффициент вытеснение</t>
+          <t>тот сера</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.08328531599620162</v>
+        <v>0.08989595439608609</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>коэффициент вытеснение коэффициент</t>
+          <t>ун тот сера, тот сера география</t>
         </is>
       </c>
     </row>
@@ -672,17 +668,13 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>добыча нефть</t>
+          <t>ун тот сера</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.07760259722609228</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>добыча нефть казак, насос добыча нефть, технология добыча нефть</t>
-        </is>
-      </c>
+        <v>0.08989595439608609</v>
+      </c>
+      <c r="D14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -690,15 +682,15 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>вытеснение</t>
+          <t>пау</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.07368362788503983</v>
+        <v>0.08989595439608609</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>коэффициент вытеснение, коэффициент вытеснение коэффициент, вытеснение коэффициент, вытеснение коэффициент охват</t>
+          <t>ассоциация пау</t>
         </is>
       </c>
     </row>
@@ -708,13 +700,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>коэффициент охват пласт</t>
+          <t>сера география</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.06900599370267761</v>
-      </c>
-      <c r="D16" t="inlineStr"/>
+        <v>0.08989595439608609</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>тот сера география</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -722,17 +718,13 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>повышение нефтеотдача</t>
+          <t>тот сера география</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.06703596991733099</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>метод повышение нефтеотдача, повышение нефтеотдача пласт</t>
-        </is>
-      </c>
+        <v>0.08989595439608609</v>
+      </c>
+      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -740,15 +732,15 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>добыча</t>
+          <t>самоочищение</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.0664686586960473</v>
+        <v>0.08970626442700558</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>добыча нефть, добыча нефть казак, техника технология добыча, насос добыча нефть</t>
+          <t>потенциал самоочищение, самоочищение почва</t>
         </is>
       </c>
     </row>
@@ -758,15 +750,15 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>извлечь</t>
+          <t>углеводород</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.0656487220294175</v>
+        <v>0.0866672904902405</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>извлечь пласт, количество извлечь пласт, количество извлечь, извлечь пласт нефть</t>
+          <t>техногенный углеводород, углеводородный, полициклический ароматический углеводород, углеводородный геохимический</t>
         </is>
       </c>
     </row>
@@ -776,15 +768,15 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>извлечь пласт</t>
+          <t>карта</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.06366864099664031</v>
+        <v>0.08666181382866055</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>количество извлечь пласт, извлечь пласт нефть</t>
+          <t>эколого геохимический карта, геохимический карта</t>
         </is>
       </c>
     </row>
@@ -794,15 +786,15 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>бухаленко</t>
+          <t>природный</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.06366864099664031</v>
+        <v>0.08623802941483347</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>оборудование бухаленко, нефтепромысловый оборудование бухаленко</t>
+          <t>природный среда, природный техногенный, нефтепродукт природный, природный техногенный поток</t>
         </is>
       </c>
     </row>
@@ -812,15 +804,15 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>муравей</t>
+          <t>ун</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.06366864099664031</v>
+        <v>0.08517805704163238</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>недра муравей</t>
+          <t>моск ун тот, моск ун, ун тот сера, ун тот</t>
         </is>
       </c>
     </row>
@@ -830,13 +822,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>фактор влиять нефтеотдача</t>
+          <t>ун тот</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.06366864099664031</v>
-      </c>
-      <c r="D23" t="inlineStr"/>
+        <v>0.08517805704163238</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>моск ун тот, ун тот сера</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -844,13 +840,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>количество извлечь пласт</t>
+          <t>тот</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.06366864099664031</v>
-      </c>
-      <c r="D24" t="inlineStr"/>
+        <v>0.08313586864282774</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>моск ун тот, тот сера, ун тот сера, тот сера география</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -858,15 +858,15 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>влиять нефтеотдача</t>
+          <t>эколого геохимический</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.06366864099664031</v>
+        <v>0.08298088098100256</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>фактор влиять нефтеотдача</t>
+          <t>эколого геохимический карта, прогнозный эколого геохимический, эколого геохимический состояние</t>
         </is>
       </c>
     </row>
@@ -876,15 +876,15 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>залежь</t>
+          <t>нефтепродукт</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.06169499622480266</v>
+        <v>0.07969188806726681</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>охват залежь заводнение, залежь заводнение, коэффициент охват залежь, охват залежь</t>
+          <t>нефть нефтепродукт, аккумуляция нефть нефтепродукт, нефтепродукт природный, содержание нефтепродукт</t>
         </is>
       </c>
     </row>
@@ -894,15 +894,15 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>охват пласт</t>
+          <t>нефть</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.06127634396227585</v>
+        <v>0.07876325837688636</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>коэффициент охват пласт, охват пласт воздействие</t>
+          <t>нефть нефтепродукт, аккумуляция нефть, аккумуляция нефть нефтепродукт, нефть окружающий среда</t>
         </is>
       </c>
     </row>
@@ -912,15 +912,15 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>геологический запас</t>
+          <t>пиковский</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.06127634396227585</v>
+        <v>0.07801777968948236</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>начальный геологический запас, геологический запас нефть</t>
+          <t>геннадий пиковский</t>
         </is>
       </c>
     </row>
@@ -930,15 +930,15 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>текущий нефтеотдача</t>
+          <t>ореол</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.06079492104294596</v>
+        <v>0.0777454291700715</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>нефтеотдача текущий нефтеотдача</t>
+          <t>ореол загрязнение, ореол нефтяной загрязнение, ореол нефтяной</t>
         </is>
       </c>
     </row>
@@ -948,15 +948,15 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>количество извлечь</t>
+          <t>вестн моск</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.06079492104294596</v>
+        <v>0.07606580756591901</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>количество извлечь пласт, отношение количество извлечь</t>
+          <t>вестн моск ун</t>
         </is>
       </c>
     </row>
@@ -966,17 +966,13 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>охватить</t>
+          <t>вестн моск ун</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.05721294839882425</v>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>пласт охватить, охватить заводнение, пласт охватить заводнение, зона охватить</t>
-        </is>
-      </c>
+        <v>0.07606580756591901</v>
+      </c>
+      <c r="D31" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add simple LDA-model (sklearn and gensim versions)
</commit_message>
<xml_diff>
--- a/data/result/result.xlsx
+++ b/data/result/result.xlsx
@@ -456,15 +456,15 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>почва</t>
+          <t>скважина</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.3885720750025864</v>
+        <v>0.2282964269090711</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>устойчивость почва, почва грунт, режим почва, самоочищение почва</t>
+          <t>добывать скважина, добывать скважина очаг, скважина очаг, нагнетательный скважина</t>
         </is>
       </c>
     </row>
@@ -474,15 +474,15 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>загрязнение</t>
+          <t>скв</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.180935045705758</v>
+        <v>0.2095315326627219</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>нефтяной загрязнение, источник загрязнение, ореол загрязнение, ореол нефтяной загрязнение</t>
+          <t>скважина, добывать скважина, добывать скважина очаг, скважина очаг</t>
         </is>
       </c>
     </row>
@@ -492,15 +492,15 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ландшафт</t>
+          <t>очаг</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.1449324059469544</v>
+        <v>0.2027955808466008</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>компонент ландшафт, ландшафтно геохимический, ландшафтно, состояние ландшафт</t>
+          <t>очаг нагнетание, добывать скважина очаг, скважина очаг, очаг скв</t>
         </is>
       </c>
     </row>
@@ -510,15 +510,15 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>геохимический</t>
+          <t>заводнение</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.1381817999887385</v>
+        <v>0.1676252261301775</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>эколого геохимический, эколого геохимический карта, геохимический поле, ландшафтно геохимический</t>
+          <t>эффективность заводнение, процесс заводнение, оценка эффективность заводнение, заводнение различный</t>
         </is>
       </c>
     </row>
@@ -528,15 +528,15 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>поллютант</t>
+          <t>значение</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.1365767393522176</v>
+        <v>0.1285799401740974</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>поллютант природный</t>
+          <t>изменение значение, значение коэффициент, значение очаг, изменение значение коэффициент</t>
         </is>
       </c>
     </row>
@@ -546,15 +546,15 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>почвенный</t>
+          <t>очаг нагнетание</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.1084635580499261</v>
+        <v>0.128566652808574</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>почвенный покров, почвенный экосистема</t>
+          <t>очаг нагнетание скв, очаг нагнетание скважина</t>
         </is>
       </c>
     </row>
@@ -564,13 +564,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>моск ун тот</t>
+          <t>изменение значение</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.1037261012262532</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
+        <v>0.1257527682755146</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>изменение значение коэффициент, изменение значение скважина, скважина изменение значение</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -578,15 +582,15 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>моск ун</t>
+          <t>коэффициент</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.1037261012262532</v>
+        <v>0.1071038628702217</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>моск ун тот, вестн моск ун, во моск ун</t>
+          <t>значение коэффициент, изменение коэффициент проницаемость, изменение коэффициент, коэффициент проницаемость</t>
         </is>
       </c>
     </row>
@@ -596,15 +600,15 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>моск</t>
+          <t>зарифовый мелководье</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.09752222461185295</v>
+        <v>0.1051908977524696</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>моск ун тот, моск ун, вестн моск, вестн моск ун</t>
+          <t>зона зарифовый мелководье, зарифовый мелководье рифовый</t>
         </is>
       </c>
     </row>
@@ -614,15 +618,15 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>география</t>
+          <t>зарифовый</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.09589309825489614</v>
+        <v>0.1051908977524696</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>сера география, тот сера география</t>
+          <t>зарифовый мелководье, зона зарифовый, зона зарифовый мелководье, фациальный зона зарифовый</t>
         </is>
       </c>
     </row>
@@ -632,15 +636,15 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>техногенный</t>
+          <t>эффективность заводнение</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.0955063826114305</v>
+        <v>0.1004430473651141</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>техногенный углеводород, техногенный поток, техногенный поток углеводород, природный техногенный</t>
+          <t>оценка эффективность заводнение</t>
         </is>
       </c>
     </row>
@@ -650,15 +654,15 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>тот сера</t>
+          <t>добывать скважина</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.08989595439608609</v>
+        <v>0.09543863365683752</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ун тот сера, тот сера география</t>
+          <t>добывать скважина очаг, коэффициент добывать скважина, фронт добывать скважина</t>
         </is>
       </c>
     </row>
@@ -668,13 +672,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ун тот сера</t>
+          <t>закачка</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.08989595439608609</v>
-      </c>
-      <c r="D14" t="inlineStr"/>
+        <v>0.09518957143501156</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>накопить закачка, закачка рабочий агент, закачка рабочий, нефть накопить закачка</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -682,15 +690,15 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>пау</t>
+          <t>добывать</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.08989595439608609</v>
+        <v>0.09469509279688046</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>ассоциация пау</t>
+          <t>добывать скважина, добывать скважина очаг, скважина добывать, коэффициент добывать</t>
         </is>
       </c>
     </row>
@@ -700,15 +708,15 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>сера география</t>
+          <t>рифовый</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.08989595439608609</v>
+        <v>0.08900347769826436</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>тот сера география</t>
+          <t>зарифовый мелководье, зарифовый, рифовый гребень, зона зарифовый</t>
         </is>
       </c>
     </row>
@@ -718,13 +726,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>тот сера география</t>
+          <t>нагнетание</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.08989595439608609</v>
-      </c>
-      <c r="D17" t="inlineStr"/>
+        <v>0.08381261306508876</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>очаг нагнетание, очаг нагнетание скв, нагнетание скв, очаг нагнетание скважина</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -732,15 +744,15 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>самоочищение</t>
+          <t>значение коэффициент</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.08970626442700558</v>
+        <v>0.08325549266051276</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>потенциал самоочищение, самоочищение почва</t>
+          <t>изменение значение коэффициент, значение коэффициент добывать</t>
         </is>
       </c>
     </row>
@@ -750,17 +762,13 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>углеводород</t>
+          <t>изменение коэффициент проницаемость</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.0866672904902405</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>техногенный углеводород, углеводородный, полициклический ароматический углеводород, углеводородный геохимический</t>
-        </is>
-      </c>
+        <v>0.08181514269636525</v>
+      </c>
+      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -768,17 +776,13 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>карта</t>
+          <t>добывать скважина очаг</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.08666181382866055</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>эколого геохимический карта, геохимический карта</t>
-        </is>
-      </c>
+        <v>0.08181514269636525</v>
+      </c>
+      <c r="D20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -786,17 +790,13 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>природный</t>
+          <t>рифовый гребень</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.08623802941483347</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>природный среда, природный техногенный, нефтепродукт природный, природный техногенный поток</t>
-        </is>
-      </c>
+        <v>0.08181514269636525</v>
+      </c>
+      <c r="D21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -804,15 +804,15 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ун</t>
+          <t>мелководье</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.08517805704163238</v>
+        <v>0.0809907487451607</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>моск ун тот, моск ун, ун тот сера, ун тот</t>
+          <t>зарифовый мелководье, зона зарифовый мелководье, мелководье рифовый, зарифовый мелководье рифовый</t>
         </is>
       </c>
     </row>
@@ -822,15 +822,15 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ун тот</t>
+          <t>фациальный зона</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.08517805704163238</v>
+        <v>0.07911420239845721</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>моск ун тот, ун тот сера</t>
+          <t>фациальный зона зарифовый</t>
         </is>
       </c>
     </row>
@@ -840,15 +840,15 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>тот</t>
+          <t>скважина очаг</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.08313586864282774</v>
+        <v>0.07812237017286656</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>моск ун тот, тот сера, ун тот сера, тот сера география</t>
+          <t>добывать скважина очаг, скважина очаг скв</t>
         </is>
       </c>
     </row>
@@ -858,15 +858,15 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>эколого геохимический</t>
+          <t>проницаемость</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.08298088098100256</v>
+        <v>0.0780524968177891</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>эколого геохимический карта, прогнозный эколого геохимический, эколого геохимический состояние</t>
+          <t>изменение коэффициент проницаемость, коэффициент проницаемость</t>
         </is>
       </c>
     </row>
@@ -876,15 +876,15 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>нефтепродукт</t>
+          <t>изменение коэффициент</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.07969188806726681</v>
+        <v>0.07738631893877819</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>нефть нефтепродукт, аккумуляция нефть нефтепродукт, нефтепродукт природный, содержание нефтепродукт</t>
+          <t>изменение коэффициент проницаемость</t>
         </is>
       </c>
     </row>
@@ -894,15 +894,15 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>нефть</t>
+          <t>нагнетательный</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.07876325837688636</v>
+        <v>0.07685286067135809</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>нефть нефтепродукт, аккумуляция нефть, аккумуляция нефть нефтепродукт, нефть окружающий среда</t>
+          <t>нагнетательный скважина, нагнетательный скважина добывать, фронт нагнетать нагнетательный</t>
         </is>
       </c>
     </row>
@@ -912,15 +912,15 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>пиковский</t>
+          <t>гребень</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.07801777968948236</v>
+        <v>0.07525803327461529</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>геннадий пиковский</t>
+          <t>рифовый гребень</t>
         </is>
       </c>
     </row>
@@ -930,15 +930,15 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ореол</t>
+          <t>озёрный</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.0777454291700715</v>
+        <v>0.07291769962214874</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>ореол загрязнение, ореол нефтяной загрязнение, ореол нефтяной</t>
+          <t>озёрный месторождение, фм озёрный месторождение, фм озёрный</t>
         </is>
       </c>
     </row>
@@ -948,15 +948,15 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>вестн моск</t>
+          <t>фациальный</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.07606580756591901</v>
+        <v>0.07230820802285964</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>вестн моск ун</t>
+          <t>фациальный зона, фациальный зона зарифовый</t>
         </is>
       </c>
     </row>
@@ -966,13 +966,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>вестн моск ун</t>
+          <t>изменение</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.07606580756591901</v>
-      </c>
-      <c r="D31" t="inlineStr"/>
+        <v>0.07055046159262758</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>изменение значение, изменение коэффициент проницаемость, изменение коэффициент, скважина изменение</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add new function into processing
</commit_message>
<xml_diff>
--- a/data/result/result.xlsx
+++ b/data/result/result.xlsx
@@ -456,15 +456,15 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>нефтеотдача</t>
+          <t>почва</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.3288214439537894</v>
+        <v>0.3881364042388271</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>конечный нефтеотдача, нефтеотдача пласт, повышение нефтеотдача, фактор влиять нефтеотдача</t>
+          <t>устойчивость почва, почва грунт, самоочищение почва, режим почва</t>
         </is>
       </c>
     </row>
@@ -474,15 +474,15 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>пласт</t>
+          <t>загрязнение</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.2020149243149546</v>
+        <v>0.1807321795848384</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>нефтеотдача пласт, коэффициент охват пласт, извлечь пласт, количество извлечь пласт</t>
+          <t>нефтяной загрязнение, источник загрязнение, ореол нефтяной загрязнение, ореол загрязнение</t>
         </is>
       </c>
     </row>
@@ -492,15 +492,15 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>нефть</t>
+          <t>ландшафт</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.178806955663011</v>
+        <v>0.1447699063334863</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>добыча нефть, вязкость нефть, извлечь пласт нефть, нефть пласт</t>
+          <t>компонент ландшафт, ландшафтно геохимический, ландшафтно, устойчивость ландшафт</t>
         </is>
       </c>
     </row>
@@ -510,15 +510,15 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>заводнение</t>
+          <t>геохимический</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.1141403809079946</v>
+        <v>0.1380268692198758</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>охват залежь заводнение, залежь заводнение, заводнение коэффициент, заводнение коэффициент охват</t>
+          <t>эколого геохимический, углеводородный геохимический, углеводородный геохимический поле, геохимический поле</t>
         </is>
       </c>
     </row>
@@ -528,15 +528,15 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>коэффициент охват</t>
+          <t>поллютант</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.1053887189256356</v>
+        <v>0.136423608192844</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>коэффициент охват пласт, заводнение коэффициент охват, коэффициент охват залежь, вытеснение коэффициент охват</t>
+          <t>поллютант природный</t>
         </is>
       </c>
     </row>
@@ -546,15 +546,15 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>конечный нефтеотдача</t>
+          <t>почвенный</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.09660839118374866</v>
+        <v>0.1083419476609774</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>конечный нефтеотдача текущий</t>
+          <t>почвенный покров, почвенный экосистема</t>
         </is>
       </c>
     </row>
@@ -564,15 +564,15 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>отношение количество</t>
+          <t>моск ун</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.09550296149496046</v>
+        <v>0.1036098025196549</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>нефтеотдача отношение количество, отношение количество извлечь</t>
+          <t>моск ун тот, вестн моск ун, во моск ун</t>
         </is>
       </c>
     </row>
@@ -582,17 +582,13 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>коэффициент</t>
+          <t>моск ун тот</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.09237775791152383</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>коэффициент охват, коэффициент вытеснение, коэффициент охват пласт, коэффициент вытеснение коэффициент</t>
-        </is>
-      </c>
+        <v>0.1036098025196549</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -600,15 +596,15 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>нефтеотдача пласт</t>
+          <t>моск</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.09076514308339242</v>
+        <v>0.09741288175163872</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>повышение нефтеотдача пласт</t>
+          <t>моск ун, моск ун тот, вестн моск, вестн моск ун</t>
         </is>
       </c>
     </row>
@@ -618,15 +614,15 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>недра</t>
+          <t>география</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.08559366195950284</v>
+        <v>0.09578558198688926</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>недра муравей, недра казак</t>
+          <t>сера география, тот сера география</t>
         </is>
       </c>
     </row>
@@ -636,15 +632,15 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>охват</t>
+          <t>техногенный</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.08497771763711093</v>
+        <v>0.09539929993273841</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>коэффициент охват, коэффициент охват пласт, охват пласт, охватить</t>
+          <t>техногенный поток, техногенный углеводород, техногенный поток углеводород, природный техногенный</t>
         </is>
       </c>
     </row>
@@ -654,15 +650,15 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>коэффициент вытеснение</t>
+          <t>сера география</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.08328531599620162</v>
+        <v>0.08979516218370089</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>коэффициент вытеснение коэффициент</t>
+          <t>тот сера география</t>
         </is>
       </c>
     </row>
@@ -672,15 +668,15 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>добыча нефть</t>
+          <t>пау</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.07760259722609228</v>
+        <v>0.08979516218370089</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>добыча нефть казак, насос добыча нефть, технология добыча нефть</t>
+          <t>ассоциация пау</t>
         </is>
       </c>
     </row>
@@ -690,17 +686,13 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>вытеснение</t>
+          <t>ун тот сера</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.07368362788503983</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>коэффициент вытеснение, коэффициент вытеснение коэффициент, вытеснение коэффициент, вытеснение коэффициент охват</t>
-        </is>
-      </c>
+        <v>0.08979516218370089</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -708,13 +700,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>коэффициент охват пласт</t>
+          <t>тот сера</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.06900599370267761</v>
-      </c>
-      <c r="D16" t="inlineStr"/>
+        <v>0.08979516218370089</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>ун тот сера, тот сера география</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -722,17 +718,13 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>повышение нефтеотдача</t>
+          <t>тот сера география</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.06703596991733099</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>метод повышение нефтеотдача, повышение нефтеотдача пласт</t>
-        </is>
-      </c>
+        <v>0.08979516218370089</v>
+      </c>
+      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -740,15 +732,15 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>добыча</t>
+          <t>самоочищение</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.0664686586960473</v>
+        <v>0.08960568489684594</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>добыча нефть, добыча нефть казак, техника технология добыча, насос добыча нефть</t>
+          <t>потенциал самоочищение, самоочищение почва</t>
         </is>
       </c>
     </row>
@@ -758,15 +750,15 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>извлечь</t>
+          <t>углеводород</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.0656487220294175</v>
+        <v>0.08657011828701258</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>извлечь пласт, количество извлечь пласт, количество извлечь, извлечь пласт нефть</t>
+          <t>техногенный углеводород, углеводородный, полициклический ароматический углеводород, углеводородный геохимический</t>
         </is>
       </c>
     </row>
@@ -776,15 +768,15 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>извлечь пласт</t>
+          <t>карта</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.06366864099664031</v>
+        <v>0.0865646477659185</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>количество извлечь пласт, извлечь пласт нефть</t>
+          <t>эколого геохимический карта, геохимический карта</t>
         </is>
       </c>
     </row>
@@ -794,15 +786,15 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>бухаленко</t>
+          <t>природный</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.06366864099664031</v>
+        <v>0.08614133850326959</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>оборудование бухаленко, нефтепромысловый оборудование бухаленко</t>
+          <t>природный среда, природный техногенный, природный техногенный поток, поллютант природный</t>
         </is>
       </c>
     </row>
@@ -812,15 +804,15 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>муравей</t>
+          <t>ун</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.06366864099664031</v>
+        <v>0.08508255458133174</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>недра муравей</t>
+          <t>моск ун, моск ун тот, ун тот сера, ун тот</t>
         </is>
       </c>
     </row>
@@ -830,13 +822,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>фактор влиять нефтеотдача</t>
+          <t>ун тот</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.06366864099664031</v>
-      </c>
-      <c r="D23" t="inlineStr"/>
+        <v>0.08508255458133174</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>моск ун тот, ун тот сера</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -844,13 +840,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>количество извлечь пласт</t>
+          <t>тот</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.06366864099664031</v>
-      </c>
-      <c r="D24" t="inlineStr"/>
+        <v>0.08304265590388558</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>моск ун тот, ун тот сера, тот сера, тот сера география</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -858,15 +858,15 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>влиять нефтеотдача</t>
+          <t>эколого геохимический</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.06366864099664031</v>
+        <v>0.0828878420157239</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>фактор влиять нефтеотдача</t>
+          <t>эколого геохимический карта, прогнозный эколого геохимический, эколого геохимический состояние</t>
         </is>
       </c>
     </row>
@@ -876,15 +876,15 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>залежь</t>
+          <t>нефтепродукт</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.06169499622480266</v>
+        <v>0.07960253675261182</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>охват залежь заводнение, залежь заводнение, коэффициент охват залежь, охват залежь</t>
+          <t>нефть нефтепродукт, аккумуляция нефть нефтепродукт, нефтепродукт природный, содержание нефтепродукт</t>
         </is>
       </c>
     </row>
@@ -894,15 +894,15 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>охват пласт</t>
+          <t>нефть</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.06127634396227585</v>
+        <v>0.07867494825080998</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>коэффициент охват пласт, охват пласт воздействие</t>
+          <t>нефть нефтепродукт, аккумуляция нефть, аккумуляция нефть нефтепродукт, нефть окружающий среда</t>
         </is>
       </c>
     </row>
@@ -912,15 +912,15 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>геологический запас</t>
+          <t>пиковский</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.06127634396227585</v>
+        <v>0.07793030540131098</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>начальный геологический запас, геологический запас нефть</t>
+          <t>геннадий пиковский</t>
         </is>
       </c>
     </row>
@@ -930,15 +930,15 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>текущий нефтеотдача</t>
+          <t>ореол</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.06079492104294596</v>
+        <v>0.07765826024393314</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>нефтеотдача текущий нефтеотдача</t>
+          <t>ореол нефтяной загрязнение, ореол нефтяной, ореол загрязнение</t>
         </is>
       </c>
     </row>
@@ -948,15 +948,15 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>количество извлечь</t>
+          <t>вестн моск</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.06079492104294596</v>
+        <v>0.07598052184774691</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>количество извлечь пласт, отношение количество извлечь</t>
+          <t>вестн моск ун</t>
         </is>
       </c>
     </row>
@@ -966,17 +966,13 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>охватить</t>
+          <t>вестн моск ун</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.05721294839882425</v>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>пласт охватить, охватить заводнение, пласт охватить заводнение, зона охватить</t>
-        </is>
-      </c>
+        <v>0.07598052184774691</v>
+      </c>
+      <c r="D31" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>